<commit_message>
doc version for sub2
</commit_message>
<xml_diff>
--- a/202010_jslhr/tables.xlsx
+++ b/202010_jslhr/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10440" yWindow="1380" windowWidth="27320" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="1800" windowWidth="27320" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Recall</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Zoon.</t>
   </si>
   <si>
-    <t>Lab</t>
-  </si>
-  <si>
     <t>Crying</t>
   </si>
   <si>
@@ -63,6 +60,72 @@
   </si>
   <si>
     <t>WAR</t>
+  </si>
+  <si>
+    <t>table 1</t>
+  </si>
+  <si>
+    <t>tablé 2</t>
+  </si>
+  <si>
+    <t>Linguistic Proportion</t>
+  </si>
+  <si>
+    <t>Canonical Proportion</t>
+  </si>
+  <si>
+    <t>All seg AS</t>
+  </si>
+  <si>
+    <t>Chunks AS</t>
+  </si>
+  <si>
+    <t>100 seg AS</t>
+  </si>
+  <si>
+    <t>All seg LR</t>
+  </si>
+  <si>
+    <t>Chunks LR</t>
+  </si>
+  <si>
+    <t>100 seg LR</t>
+  </si>
+  <si>
+    <t>All seg all</t>
+  </si>
+  <si>
+    <t>Chunks all</t>
+  </si>
+  <si>
+    <t>100 seg all</t>
+  </si>
+  <si>
+    <t>table 3</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>LP (lab)</t>
+  </si>
+  <si>
+    <t>LP (Zoon. Seg.)</t>
+  </si>
+  <si>
+    <t>LP (Zoon. Chunks)</t>
+  </si>
+  <si>
+    <t>CP (lab)</t>
+  </si>
+  <si>
+    <t>CP (Zoon. Seg.)</t>
+  </si>
+  <si>
+    <t>CP (Zoon. Chunks)</t>
   </si>
 </sst>
 </file>
@@ -116,8 +179,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -130,20 +201,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25:P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,168 +510,368 @@
     <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="3">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="C3" s="3">
+        <v>78</v>
+      </c>
+      <c r="D3" s="3">
+        <v>50.9</v>
+      </c>
+      <c r="E3" s="3">
+        <v>669</v>
+      </c>
+      <c r="F3" s="3">
+        <v>6762</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
-        <v>70.599999999999994</v>
-      </c>
-      <c r="C3" s="1">
-        <v>78</v>
-      </c>
-      <c r="D3" s="1">
-        <v>49</v>
-      </c>
-      <c r="E3" s="1">
-        <v>669</v>
-      </c>
-      <c r="F3" s="1">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="3">
+        <v>41.5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3">
+        <v>62.9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>149</v>
+      </c>
+      <c r="F4" s="3">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
-        <v>41.5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1">
-        <v>149</v>
-      </c>
-      <c r="F4" s="1">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="3">
+        <v>24.1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>77</v>
+      </c>
+      <c r="D5" s="3">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="E5" s="3">
+        <v>4485</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
-        <v>24.1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>73</v>
-      </c>
-      <c r="D5" s="1">
-        <v>77</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4485</v>
-      </c>
-      <c r="F5" s="1">
-        <v>5512</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="3">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="C6" s="3">
+        <v>59</v>
+      </c>
+      <c r="D6" s="3">
+        <v>58.3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1426</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
-        <v>66.400000000000006</v>
-      </c>
-      <c r="C6" s="1">
-        <v>73</v>
-      </c>
-      <c r="D6" s="1">
-        <v>59</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1426</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1715</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="3">
+        <v>67.3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>43.5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4575</v>
+      </c>
+      <c r="F7" s="3">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1">
-        <v>67.3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>44</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4575</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="3">
+        <v>54</v>
+      </c>
+      <c r="C8" s="3">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3">
+        <v>58.9</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1">
-        <v>54</v>
-      </c>
-      <c r="C8" s="1">
-        <v>41</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="B9" s="3">
+        <v>49.9</v>
+      </c>
+      <c r="C9" s="3">
         <v>57</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1">
-        <v>49.9</v>
-      </c>
-      <c r="C9" s="1">
-        <v>57</v>
-      </c>
-      <c r="D9" s="1">
-        <v>65</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="D9" s="3">
+        <v>55.3</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.63200000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="I17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.83</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.96599999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="I18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.97399999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="I19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="I20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="I21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.96299999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="I22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.90500000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="M24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="N25" s="3"/>
+      <c r="O25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="N26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O26" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P26" s="3">
+        <v>0.74099999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="N27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="3">
+        <v>-0.13100000000000001</v>
+      </c>
+      <c r="P27" s="3">
+        <v>0.67200000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="N28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O28" s="3">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0.71599999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="N29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O29" s="3">
+        <v>-0.55700000000000005</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0.60699999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="N30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O30" s="3">
+        <v>-0.40400000000000003</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0.60399999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="N31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O31" s="3">
+        <v>-0.38</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0.57299999999999995</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>